<commit_message>
Setting Emission values to zero for  non emission fuel. New look up table.
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Caption_Table.xlsx
+++ b/TIMES_shiny/data_cleaning/Caption_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
   <si>
     <t>Subsector</t>
   </si>
@@ -270,6 +270,27 @@
   </si>
   <si>
     <t>Emissions from international shipping are not constraint in the model.</t>
+  </si>
+  <si>
+    <t>All Other Subsectors</t>
+  </si>
+  <si>
+    <t>All Agriculture Subsectors</t>
+  </si>
+  <si>
+    <t>All Residential Subsectors</t>
+  </si>
+  <si>
+    <t>All Commercial Subsectors</t>
+  </si>
+  <si>
+    <t>All Industry Subsectors</t>
+  </si>
+  <si>
+    <t>All Transport Subsectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Draft commentary: The scenario shows that petrol has high consumption until 2035 at which point in sharply decreases  </t>
   </si>
 </sst>
 </file>
@@ -596,16 +617,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="184.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -626,7 +647,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
@@ -634,15 +655,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -650,7 +671,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
@@ -658,7 +679,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>46</v>
@@ -666,7 +687,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
@@ -674,265 +695,313 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>15</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B47" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
About page content and tons of modifications
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Caption_Table.xlsx
+++ b/TIMES_shiny/data_cleaning/Caption_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="104">
   <si>
     <t>Subsector</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Healthcare</t>
   </si>
   <si>
-    <t>Horticulture</t>
-  </si>
-  <si>
     <t>Hydro</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>Livestock farming is not expected to grow much because of land constraints, and energy productivity improvements (mostly in) irrigation cause reductions in energy demand.</t>
   </si>
   <si>
-    <t>This balances energy in according to New Zealand's Energy Balances from MBIE.</t>
-  </si>
-  <si>
     <t>Commercial</t>
   </si>
   <si>
@@ -218,18 +212,9 @@
     <t>Coal and Natural Gas decrease significantly as new wind and hydro generation gets developed. Natural Gas is supplied during winter months due to the limited amount of other economically achievable options</t>
   </si>
   <si>
-    <t xml:space="preserve">Wind grows faster in Tui as the Aluminium smelter exit in Kea results in less electricity demand for Kea. </t>
-  </si>
-  <si>
     <t>Industrial</t>
   </si>
   <si>
-    <t>Large decarbonisation occurs in the industrial sector with most of the remaining fossil fuels in hard to abate sectors. Additionally, biofuels would reduce the remaining diesel emissions by 40%</t>
-  </si>
-  <si>
-    <t>In Kea, aluminium smelting reaches zero in 2030, and in Tui the demand stays as the smelter may continue to run or is replaced by another industry.</t>
-  </si>
-  <si>
     <t>Diesel prolongs in both scenarios as alternative technologies are not yet available. There is 4 PJ of biofuel in Kea further reducing diesel emissions</t>
   </si>
   <si>
@@ -239,12 +224,6 @@
     <t xml:space="preserve">Coal for process heat gets replaced by biomass in both scenarios but at different rates. </t>
   </si>
   <si>
-    <t>Fabricated Metal Products, Transport Equipment, Machinery and Equipment Manufacturing</t>
-  </si>
-  <si>
-    <t>Tui assumes a higher growth rate than in Kea, because Kea tries to move away from emission-heavy manufacturing.</t>
-  </si>
-  <si>
     <t>Both scenarios assume a constant energy demand, with natural gas used for process heat being displaced.</t>
   </si>
   <si>
@@ -254,9 +233,6 @@
     <t xml:space="preserve">Coal for process heat gets replaced by heat pumps for hot water in both scenarios but at different rates. </t>
   </si>
   <si>
-    <t xml:space="preserve">Kea assumes methanol production exits at 2032.  In Tui it exits in 2047. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Diesel prolongs in both scenarios as alternative technologies are not yet available. There is 2.3 PJ of biofuel in Kea further reducing diesel emissions </t>
   </si>
   <si>
@@ -317,16 +293,49 @@
     <t>Transport</t>
   </si>
   <si>
-    <t>A strong drive for electrification reduces emissions significantly. Tui sees greater use of hybrids in the short term, while Kea pushes hard on EVs.</t>
-  </si>
-  <si>
     <t>Emissions from international aviation are not constrained in the model. Fuel consumption for aviation decreases in the period 2045-2060 because the Kea scenario assumes an aspect of flight shame.</t>
   </si>
   <si>
     <t>Road Transport</t>
   </si>
   <si>
-    <t>In each time period, the share of EVs is larger in Kea than in Tui because the Kea scenario assumes there is a larger ability to access EVs.</t>
+    <t xml:space="preserve">Wind grows faster in Tūī as the Aluminium smelter exit in Kea results in less electricity demand for Kea. </t>
+  </si>
+  <si>
+    <t>In Kea, aluminium smelting reaches zero in 2030, and in Tūī the demand stays as the smelter may continue to run or is replaced by another industry.</t>
+  </si>
+  <si>
+    <t>Tūī assumes a higher growth rate than in Kea, because Kea tries to move away from emission-heavy manufacturing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kea assumes methanol production exits at 2032.  In Tūī it exits in 2047. </t>
+  </si>
+  <si>
+    <t>A strong drive for electrification reduces emissions significantly. Tūī sees greater use of hybrids in the short term, while Kea pushes hard on EVs.</t>
+  </si>
+  <si>
+    <t>Fabricated Metal Product, Transport Equipment, Machinery and Equipment Manufacturing</t>
+  </si>
+  <si>
+    <t>Other (Agriculture)</t>
+  </si>
+  <si>
+    <t>Other (Commercial)</t>
+  </si>
+  <si>
+    <t>Other (Industry)</t>
+  </si>
+  <si>
+    <t>Outdoor Horticulture/Arable Farming</t>
+  </si>
+  <si>
+    <t>Large decarbonisation occurs in the industrial sector with most of the remaining fossil fuels in hard to abate sectors. Note - Only energy related emissions are included in the TIMES-NZ model. Emissions from Feedstock are not expressed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In each time period, the share of EVs is larger in Kea than in Tūī because the Kea scenario assumes there is a larger ability to access EVs.  Note - the end use demand for Road Transport is measured as Distance Travelled in the metric dropdown tool.</t>
+  </si>
+  <si>
+    <t>This balances energy in according to New Zealands Energy Balances from MBIE.</t>
   </si>
 </sst>
 </file>
@@ -655,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H45" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +676,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -678,519 +687,519 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
         <v>65</v>
-      </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>